<commit_message>
adding ventilation outcome and compute all in one function
</commit_message>
<xml_diff>
--- a/data-raw/hospit-severity.xlsx
+++ b/data-raw/hospit-severity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Severity" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Hospit" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ICU" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Ventilation" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -306,7 +306,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -505,8 +505,8 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -815,8 +815,8 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>